<commit_message>
Working version that macthes PVT of new and old corelations
</commit_message>
<xml_diff>
--- a/data/PVT_Data.xlsx
+++ b/data/PVT_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjdaqua\Python\Projects\HGOR\Code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B570FA5-B437-4EF5-9B0C-2A339F768ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E183946-CC33-418D-B3E1-B814105CE97A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34545" yWindow="900" windowWidth="17940" windowHeight="13275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -975,7 +975,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="37">
   <si>
     <t>Oil API at 60 F (MSST)</t>
   </si>
@@ -1043,15 +1043,6 @@
     <t>p</t>
   </si>
   <si>
-    <t>Bg_psat</t>
-  </si>
-  <si>
-    <t>Bo_psat</t>
-  </si>
-  <si>
-    <t>visc_o_psat</t>
-  </si>
-  <si>
     <t>c_o_psat</t>
   </si>
   <si>
@@ -1080,6 +1071,21 @@
   </si>
   <si>
     <t>gamma_s</t>
+  </si>
+  <si>
+    <t>visc_o</t>
+  </si>
+  <si>
+    <t>p_res</t>
+  </si>
+  <si>
+    <t>Bo_pres</t>
+  </si>
+  <si>
+    <t>Bg_pres</t>
+  </si>
+  <si>
+    <t>Rgo</t>
   </si>
 </sst>
 </file>
@@ -1613,7 +1619,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1648,7 +1654,7 @@
         <v>0</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>10</v>
@@ -1678,44 +1684,44 @@
         <v>15</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>18</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="J2" s="10"/>
       <c r="K2" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -8883,7 +8889,7 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D2" s="42">
         <v>3405000</v>
@@ -8891,7 +8897,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D3">
         <v>2.7753999999999999</v>
@@ -8899,7 +8905,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D4" s="42">
         <v>9.9999999999999995E-7</v>
@@ -8919,15 +8925,15 @@
         <v>0</v>
       </c>
       <c r="E7" s="41" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>17</v>
@@ -8939,7 +8945,7 @@
         <v>16</v>
       </c>
       <c r="F8" s="40" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Initial test with new updated data
</commit_message>
<xml_diff>
--- a/data/PVT_Data.xlsx
+++ b/data/PVT_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjdaqua\Python\Projects\HGOR\Code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA3C2D9-C4B7-4ECE-8E62-9B96FA4FD7FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D95C52-2BC7-4AF9-8DF4-614EC7C030C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$O$156</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1040,9 +1040,6 @@
     <t>Bg</t>
   </si>
   <si>
-    <t>p</t>
-  </si>
-  <si>
     <t>c_o_psat</t>
   </si>
   <si>
@@ -1086,6 +1083,9 @@
   </si>
   <si>
     <t>Rgo</t>
+  </si>
+  <si>
+    <t>psat</t>
   </si>
 </sst>
 </file>
@@ -1619,7 +1619,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1654,7 +1654,7 @@
         <v>0</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>10</v>
@@ -1684,19 +1684,19 @@
         <v>15</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>18</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>19</v>
@@ -1705,23 +1705,23 @@
         <v>20</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J2" s="10"/>
       <c r="K2" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="N2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="O2" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -8889,7 +8889,7 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="42">
         <v>3405000</v>
@@ -8897,7 +8897,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3">
         <v>2.7753999999999999</v>
@@ -8905,7 +8905,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="42">
         <v>9.9999999999999995E-7</v>
@@ -8925,15 +8925,15 @@
         <v>0</v>
       </c>
       <c r="E7" s="41" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>17</v>
@@ -8945,7 +8945,7 @@
         <v>16</v>
       </c>
       <c r="F8" s="40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">

</xml_diff>